<commit_message>
fix if else if bug, log history in excel
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="3980" yWindow="2120" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1 Fundamentals" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="13">
   <si>
     <t>Topic</t>
   </si>
@@ -69,6 +69,13 @@
   </si>
   <si>
     <t>Index</t>
+  </si>
+  <si>
+    <t>Bug 1: if , else if, else. 
+2. Define mid = lo + (hi - lo) /2
+3. if key &lt; a[mid] , hi = mid -1;
+else if key &gt; a[mid], lo = mid + 1;
+else return mid;</t>
   </si>
 </sst>
 </file>
@@ -118,7 +125,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,6 +136,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="justify" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -408,10 +421,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -438,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>4</v>
@@ -447,7 +460,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -456,13 +469,118 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
+      <c r="D2" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D10" s="5"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D15" s="5"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D17" s="5"/>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D19" s="5"/>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D26" s="5"/>
+    </row>
+    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D28" s="5"/>
+    </row>
+    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D29" s="5"/>
+    </row>
+    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D30" s="5"/>
+    </row>
+    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D31" s="5"/>
+    </row>
+    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D32" s="5"/>
+    </row>
+    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D33" s="5"/>
+    </row>
+    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D34" s="5"/>
+    </row>
+    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D35" s="5"/>
+    </row>
+    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
+      <c r="D36" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bug analysis: if else bug
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3980" yWindow="2120" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="4360" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1 Fundamentals" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="16">
   <si>
     <t>Topic</t>
   </si>
@@ -77,12 +77,25 @@
 else if key &gt; a[mid], lo = mid + 1;
 else return mid;</t>
   </si>
+  <si>
+    <t>Bugs</t>
+  </si>
+  <si>
+    <t>Bug 1: if , else if, else. 
+If the first (if statement satisfied, the below else 
+if statement shoul not be executed. But if you Write i
+n the format like this: If expre1; if expre 2; else), 
+the second if statement will always be executed!!</t>
+  </si>
+  <si>
+    <t>BinarySearchSean</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -94,6 +107,22 @@
       <b/>
       <sz val="16"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -122,10 +151,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -138,13 +169,18 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="justify"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="justify" wrapText="1"/>
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -421,26 +457,26 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="20.83203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="44.1640625" customWidth="1"/>
-    <col min="4" max="4" width="28.83203125" customWidth="1"/>
-    <col min="5" max="5" width="28.33203125" customWidth="1"/>
-    <col min="6" max="6" width="22.1640625" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" customWidth="1"/>
+    <col min="3" max="4" width="44.1640625" customWidth="1"/>
+    <col min="5" max="5" width="28.83203125" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.1640625" customWidth="1"/>
     <col min="8" max="8" width="23.33203125" customWidth="1"/>
     <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="10" max="10" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -451,16 +487,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -468,122 +504,1197 @@
       <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C2" s="6"/>
+      <c r="D2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D3" s="5"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D4" s="5"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D6" s="5"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D7" s="5"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D8" s="5"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D9" s="5"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D10" s="5"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D11" s="5"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D13" s="5"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D15" s="5"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D17" s="5"/>
-    </row>
-    <row r="18" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D18" s="5"/>
-    </row>
-    <row r="19" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D19" s="5"/>
-    </row>
-    <row r="20" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D20" s="5"/>
-    </row>
-    <row r="21" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D21" s="5"/>
-    </row>
-    <row r="22" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D22" s="5"/>
-    </row>
-    <row r="23" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D24" s="5"/>
-    </row>
-    <row r="25" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D25" s="5"/>
-    </row>
-    <row r="26" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D26" s="5"/>
-    </row>
-    <row r="27" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D27" s="5"/>
-    </row>
-    <row r="28" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D28" s="5"/>
-    </row>
-    <row r="29" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D29" s="5"/>
-    </row>
-    <row r="30" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D30" s="5"/>
-    </row>
-    <row r="31" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D31" s="5"/>
-    </row>
-    <row r="32" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D32" s="5"/>
-    </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D33" s="5"/>
-    </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D34" s="5"/>
-    </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D35" s="5"/>
-    </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.2">
-      <c r="D36" s="5"/>
+      <c r="F2" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="7">
+        <v>42887</v>
+      </c>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
+    </row>
+    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+      <c r="I21" s="6"/>
+      <c r="J21" s="6"/>
+    </row>
+    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+    </row>
+    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C23" s="6"/>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+      <c r="I23" s="6"/>
+      <c r="J23" s="6"/>
+    </row>
+    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="6"/>
+    </row>
+    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+      <c r="I25" s="6"/>
+      <c r="J25" s="6"/>
+    </row>
+    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="6"/>
+    </row>
+    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="6"/>
+    </row>
+    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C28" s="6"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="6"/>
+    </row>
+    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+    </row>
+    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="6"/>
+    </row>
+    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="6"/>
+    </row>
+    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="6"/>
+    </row>
+    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="6"/>
+    </row>
+    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+    </row>
+    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="6"/>
+    </row>
+    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+    </row>
+    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="6"/>
+    </row>
+    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="6"/>
+    </row>
+    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="6"/>
+    </row>
+    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="6"/>
+    </row>
+    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="6"/>
+    </row>
+    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="6"/>
+    </row>
+    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+    </row>
+    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="6"/>
+    </row>
+    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="6"/>
+    </row>
+    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+    </row>
+    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="6"/>
+    </row>
+    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="6"/>
+    </row>
+    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6"/>
+    </row>
+    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+    </row>
+    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+    </row>
+    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="6"/>
+    </row>
+    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C53" s="6"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="6"/>
+    </row>
+    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C54" s="6"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="6"/>
+    </row>
+    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C55" s="6"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="6"/>
+    </row>
+    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C56" s="6"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="6"/>
+    </row>
+    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+    </row>
+    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C58" s="6"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="6"/>
+    </row>
+    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C59" s="6"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="6"/>
+    </row>
+    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C60" s="6"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="6"/>
+    </row>
+    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="6"/>
+    </row>
+    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+    </row>
+    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+    </row>
+    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+    </row>
+    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="6"/>
+    </row>
+    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+    </row>
+    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+    </row>
+    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+    </row>
+    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="6"/>
+    </row>
+    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="6"/>
+    </row>
+    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+    </row>
+    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C72" s="6"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="6"/>
+    </row>
+    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C73" s="6"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="6"/>
+    </row>
+    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C74" s="6"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="6"/>
+    </row>
+    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="6"/>
+    </row>
+    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C76" s="6"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="6"/>
+    </row>
+    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C77" s="6"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="6"/>
+    </row>
+    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+    </row>
+    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C79" s="6"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="6"/>
+    </row>
+    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C80" s="6"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="6"/>
+    </row>
+    <row r="81" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C81" s="6"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="6"/>
+    </row>
+    <row r="82" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C82" s="6"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="6"/>
+    </row>
+    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C83" s="6"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="6"/>
+    </row>
+    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C84" s="6"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="6"/>
+    </row>
+    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+    </row>
+    <row r="86" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C86" s="6"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="6"/>
+    </row>
+    <row r="87" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C87" s="6"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+    </row>
+    <row r="88" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C88" s="6"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="6"/>
+    </row>
+    <row r="89" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C89" s="6"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="6"/>
+    </row>
+    <row r="90" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C90" s="6"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="6"/>
+    </row>
+    <row r="91" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C91" s="6"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+    </row>
+    <row r="92" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C92" s="6"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+    </row>
+    <row r="93" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C93" s="6"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+    </row>
+    <row r="94" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C94" s="6"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+    </row>
+    <row r="95" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+    </row>
+    <row r="96" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C96" s="6"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+    </row>
+    <row r="97" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C97" s="6"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+    </row>
+    <row r="98" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C98" s="6"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+    </row>
+    <row r="99" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+    </row>
+    <row r="100" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C100" s="6"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="6"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+    </row>
+    <row r="101" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C101" s="6"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="6"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+    </row>
+    <row r="102" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C102" s="6"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="6"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+    </row>
+    <row r="103" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="6"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+    </row>
+    <row r="104" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C104" s="6"/>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6"/>
+      <c r="F104" s="6"/>
+      <c r="G104" s="6"/>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+    </row>
+    <row r="105" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C105" s="6"/>
+      <c r="D105" s="6"/>
+      <c r="E105" s="6"/>
+      <c r="F105" s="6"/>
+      <c r="G105" s="6"/>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+    </row>
+    <row r="106" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C106" s="6"/>
+      <c r="D106" s="6"/>
+      <c r="E106" s="6"/>
+      <c r="F106" s="6"/>
+      <c r="G106" s="6"/>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+    </row>
+    <row r="107" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C107" s="6"/>
+      <c r="D107" s="6"/>
+      <c r="E107" s="6"/>
+      <c r="F107" s="6"/>
+      <c r="G107" s="6"/>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+    </row>
+    <row r="108" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C108" s="6"/>
+      <c r="D108" s="6"/>
+      <c r="E108" s="6"/>
+      <c r="F108" s="6"/>
+      <c r="G108" s="6"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+    </row>
+    <row r="109" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C109" s="6"/>
+      <c r="D109" s="6"/>
+      <c r="E109" s="6"/>
+      <c r="F109" s="6"/>
+      <c r="G109" s="6"/>
+      <c r="H109" s="6"/>
+      <c r="I109" s="6"/>
+      <c r="J109" s="6"/>
+    </row>
+    <row r="110" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C110" s="6"/>
+      <c r="D110" s="6"/>
+      <c r="E110" s="6"/>
+      <c r="F110" s="6"/>
+      <c r="G110" s="6"/>
+      <c r="H110" s="6"/>
+      <c r="I110" s="6"/>
+      <c r="J110" s="6"/>
+    </row>
+    <row r="111" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C111" s="6"/>
+      <c r="D111" s="6"/>
+      <c r="E111" s="6"/>
+      <c r="F111" s="6"/>
+      <c r="G111" s="6"/>
+      <c r="H111" s="6"/>
+      <c r="I111" s="6"/>
+      <c r="J111" s="6"/>
+    </row>
+    <row r="112" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C112" s="6"/>
+      <c r="D112" s="6"/>
+      <c r="E112" s="6"/>
+      <c r="F112" s="6"/>
+      <c r="G112" s="6"/>
+      <c r="H112" s="6"/>
+      <c r="I112" s="6"/>
+      <c r="J112" s="6"/>
+    </row>
+    <row r="113" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C113" s="6"/>
+      <c r="D113" s="6"/>
+      <c r="E113" s="6"/>
+      <c r="F113" s="6"/>
+      <c r="G113" s="6"/>
+      <c r="H113" s="6"/>
+      <c r="I113" s="6"/>
+      <c r="J113" s="6"/>
+    </row>
+    <row r="114" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C114" s="6"/>
+      <c r="D114" s="6"/>
+      <c r="E114" s="6"/>
+      <c r="F114" s="6"/>
+      <c r="G114" s="6"/>
+      <c r="H114" s="6"/>
+      <c r="I114" s="6"/>
+      <c r="J114" s="6"/>
+    </row>
+    <row r="115" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="6"/>
+    </row>
+    <row r="116" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C116" s="6"/>
+      <c r="D116" s="6"/>
+      <c r="E116" s="6"/>
+      <c r="F116" s="6"/>
+      <c r="G116" s="6"/>
+      <c r="H116" s="6"/>
+      <c r="I116" s="6"/>
+      <c r="J116" s="6"/>
+    </row>
+    <row r="117" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C117" s="6"/>
+      <c r="D117" s="6"/>
+      <c r="E117" s="6"/>
+      <c r="F117" s="6"/>
+      <c r="G117" s="6"/>
+      <c r="H117" s="6"/>
+      <c r="I117" s="6"/>
+      <c r="J117" s="6"/>
+    </row>
+    <row r="118" spans="3:10" x14ac:dyDescent="0.2">
+      <c r="C118" s="6"/>
+      <c r="D118" s="6"/>
+      <c r="E118" s="6"/>
+      <c r="F118" s="6"/>
+      <c r="G118" s="6"/>
+      <c r="H118" s="6"/>
+      <c r="I118" s="6"/>
+      <c r="J118" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
fail to swap two objects
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
   <si>
     <t>Topic</t>
   </si>
@@ -81,15 +81,41 @@
 the second if statement will always be executed!!</t>
   </si>
   <si>
-    <t>BinarySearchSean</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Define mid = lo + (hi - lo) /2
 2. if key &lt; a[mid] , hi = mid -1;
 else if key &gt; a[mid], lo = mid + 1;
 else return mid;
 3.Test with files: java BinarySearchSean ../test/tinyW.txt &lt; ../test/tinyT.txt 
 </t>
+  </si>
+  <si>
+    <t>Java parameter transfer</t>
+  </si>
+  <si>
+    <t>BinarySearchSean
+../test/tinyW.txt
+../test/tinyT.txt</t>
+  </si>
+  <si>
+    <t>&lt;Java 入门到精通&gt; 
+Chater 5.4
+p93</t>
+  </si>
+  <si>
+    <t>Chapter 1, p46
+Algorithms 4_th
+Prof.Sedgewick &amp; Prof.Wayne</t>
+  </si>
+  <si>
+    <t>1 parameter t is a new reference variable contains the same address of argument. 
+(t == time, true)
+ &lt;t.equals(time)&gt;, true)
+ 2 change the value of t can change argument time value</t>
+  </si>
+  <si>
+    <t>t和time并非同一个引用，此处引用的意思我想是指在内存中是不是同一个time类的变量，或者说time类型的指针。
+t和time在内存中处于不同的位置, both in stack，time属于对象opt，the actual object is stored in heap。
+而t属于函数 void objectMethod的Frame里，当调用结束后，t会消失。下面例子中的t1，t2，皆属于opt.swap方法中的参数，当调用时处在opt.swapFrame里，调用结束后消失。</t>
   </si>
 </sst>
 </file>
@@ -463,8 +489,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:J118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,27 +550,43 @@
         <v>13</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G2" s="8">
         <v>42887</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C3" s="7"/>
+      <c r="J2" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="240" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="E3" s="6" t="s">
+        <v>20</v>
+      </c>
       <c r="F3" s="7"/>
-      <c r="G3" s="7"/>
+      <c r="G3" s="8">
+        <v>42887</v>
+      </c>
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="7"/>
+      <c r="J3" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C4" s="7"/>

</xml_diff>

<commit_message>
practice 1 Binary Search
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4360" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1 Fundamentals" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
   <si>
     <t>Topic</t>
   </si>
@@ -116,6 +116,9 @@
     <t>t和time并非同一个引用，此处引用的意思我想是指在内存中是不是同一个time类的变量，或者说time类型的指针。
 t和time在内存中处于不同的位置, both in stack，time属于对象opt，the actual object is stored in heap。
 而t属于函数 void objectMethod的Frame里，当调用结束后，t会消失。下面例子中的t1，t2，皆属于opt.swap方法中的参数，当调用时处在opt.swapFrame里，调用结束后消失。</t>
+  </si>
+  <si>
+    <t xml:space="preserve">while (lo &lt;= hi) </t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -545,7 +548,9 @@
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="7" t="s">
+        <v>21</v>
+      </c>
       <c r="D2" s="6" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
Java test3 public non static method used in the outer class
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -74,13 +74,6 @@
     <t>Bugs</t>
   </si>
   <si>
-    <t>Bug 1: if , else if, else. 
-If the first (if statement satisfied, the below else 
-if statement shoul not be executed. But if you Write i
-n the format like this: If expre1; if expre 2; else), 
-the second if statement will always be executed!!</t>
-  </si>
-  <si>
     <t xml:space="preserve">1. Define mid = lo + (hi - lo) /2
 2. if key &lt; a[mid] , hi = mid -1;
 else if key &gt; a[mid], lo = mid + 1;
@@ -119,6 +112,14 @@
   </si>
   <si>
     <t xml:space="preserve">while (lo &lt;= hi) </t>
+  </si>
+  <si>
+    <t>Bug 1: if , else if, else. 
+If the first (if statement satisfied, the below else 
+if statement shoul not be executed. But if you Write i
+n the format like this: If expre1; if expre 2; else), 
+the second if statement will always be executed!!
+Bug 2: hi = array.length - 1;</t>
   </si>
 </sst>
 </file>
@@ -549,16 +550,16 @@
         <v>10</v>
       </c>
       <c r="C2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="G2" s="8">
         <v>42887</v>
@@ -566,7 +567,7 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="240" x14ac:dyDescent="0.2">
@@ -574,14 +575,14 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D3" s="7"/>
       <c r="E3" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F3" s="7"/>
       <c r="G3" s="8">
@@ -590,7 +591,7 @@
       <c r="H3" s="7"/>
       <c r="I3" s="7"/>
       <c r="J3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed Capacity Array Based String Stack 1
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17480" tabRatio="500"/>
+    <workbookView xWindow="1520" yWindow="440" windowWidth="25980" windowHeight="15300" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="1 Fundamentals" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="27">
   <si>
     <t>Topic</t>
   </si>
@@ -120,6 +120,29 @@
 n the format like this: If expre1; if expre 2; else), 
 the second if statement will always be executed!!
 Bug 2: hi = array.length - 1;</t>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>Fixed Capacity Stack
+Of Strings</t>
+  </si>
+  <si>
+    <t>ObjectParamTransfe.java
+ObjectParamTransfe2.java</t>
+  </si>
+  <si>
+    <t>FixedCapacityStackOfStringsSean
+.java</t>
+  </si>
+  <si>
+    <t>Stack implement based on Fixed Capocity of Array
+Pros:
+if you know that your stacks will never exceed a certain size, it works well.
+Cons:
+a user should not have to specify a maximum size for a stack;
+since there is a maximum capacity here, we need an isFull() method to go with it.</t>
   </si>
 </sst>
 </file>
@@ -187,7 +210,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -210,6 +233,9 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -491,111 +517,117 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:K118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="3"/>
-    <col min="2" max="2" width="20.83203125" style="4" customWidth="1"/>
-    <col min="3" max="4" width="44.1640625" customWidth="1"/>
-    <col min="5" max="5" width="28.83203125" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="22.1640625" customWidth="1"/>
-    <col min="8" max="8" width="23.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.5" customWidth="1"/>
-    <col min="10" max="10" width="23.83203125" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" style="3"/>
+    <col min="3" max="3" width="24.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="44" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.1640625" customWidth="1"/>
+    <col min="6" max="6" width="33.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.33203125" customWidth="1"/>
+    <col min="8" max="8" width="22.1640625" customWidth="1"/>
+    <col min="9" max="9" width="23.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.5" customWidth="1"/>
+    <col min="11" max="11" width="23.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="1" customFormat="1" ht="31" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="114" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+    <row r="2" spans="1:11" ht="114" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="C2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="G2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="G2" s="8">
+      <c r="H2" s="8">
         <v>42887</v>
       </c>
-      <c r="H2" s="7"/>
       <c r="I2" s="7"/>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7"/>
+      <c r="K2" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="240" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+    <row r="3" spans="1:11" ht="208" x14ac:dyDescent="0.2">
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="7"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="7"/>
+      <c r="F3" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="7"/>
-      <c r="G3" s="8">
+      <c r="G3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="8">
         <v>42887</v>
       </c>
-      <c r="H3" s="7"/>
       <c r="I3" s="7"/>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="7"/>
+      <c r="K3" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C4" s="7"/>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
@@ -603,19 +635,31 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
+      <c r="K4" s="7"/>
+    </row>
+    <row r="5" spans="1:11" ht="160" x14ac:dyDescent="0.2">
+      <c r="B5" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>26</v>
+      </c>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
+      <c r="G5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="H5" s="8">
+        <v>42890</v>
+      </c>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C6" s="7"/>
+      <c r="K5" s="7"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D6" s="7"/>
       <c r="E6" s="7"/>
       <c r="F6" s="7"/>
@@ -623,9 +667,9 @@
       <c r="H6" s="7"/>
       <c r="I6" s="7"/>
       <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C7" s="7"/>
+      <c r="K6" s="7"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D7" s="7"/>
       <c r="E7" s="7"/>
       <c r="F7" s="7"/>
@@ -633,9 +677,9 @@
       <c r="H7" s="7"/>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C8" s="7"/>
+      <c r="K7" s="7"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D8" s="7"/>
       <c r="E8" s="7"/>
       <c r="F8" s="7"/>
@@ -643,9 +687,9 @@
       <c r="H8" s="7"/>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C9" s="7"/>
+      <c r="K8" s="7"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D9" s="7"/>
       <c r="E9" s="7"/>
       <c r="F9" s="7"/>
@@ -653,9 +697,9 @@
       <c r="H9" s="7"/>
       <c r="I9" s="7"/>
       <c r="J9" s="7"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C10" s="7"/>
+      <c r="K9" s="7"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D10" s="7"/>
       <c r="E10" s="7"/>
       <c r="F10" s="7"/>
@@ -663,9 +707,9 @@
       <c r="H10" s="7"/>
       <c r="I10" s="7"/>
       <c r="J10" s="7"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C11" s="7"/>
+      <c r="K10" s="7"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7"/>
@@ -673,9 +717,9 @@
       <c r="H11" s="7"/>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C12" s="7"/>
+      <c r="K11" s="7"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
       <c r="F12" s="7"/>
@@ -683,9 +727,9 @@
       <c r="H12" s="7"/>
       <c r="I12" s="7"/>
       <c r="J12" s="7"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C13" s="7"/>
+      <c r="K12" s="7"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -693,9 +737,9 @@
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C14" s="7"/>
+      <c r="K13" s="7"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D14" s="7"/>
       <c r="E14" s="7"/>
       <c r="F14" s="7"/>
@@ -703,9 +747,9 @@
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
       <c r="J14" s="7"/>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C15" s="7"/>
+      <c r="K14" s="7"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
@@ -713,9 +757,9 @@
       <c r="H15" s="7"/>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C16" s="7"/>
+      <c r="K15" s="7"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="D16" s="7"/>
       <c r="E16" s="7"/>
       <c r="F16" s="7"/>
@@ -723,9 +767,9 @@
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
-    </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C17" s="7"/>
+      <c r="K16" s="7"/>
+    </row>
+    <row r="17" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D17" s="7"/>
       <c r="E17" s="7"/>
       <c r="F17" s="7"/>
@@ -733,9 +777,9 @@
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
       <c r="J17" s="7"/>
-    </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C18" s="7"/>
+      <c r="K17" s="7"/>
+    </row>
+    <row r="18" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D18" s="7"/>
       <c r="E18" s="7"/>
       <c r="F18" s="7"/>
@@ -743,9 +787,9 @@
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
-    </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C19" s="7"/>
+      <c r="K18" s="7"/>
+    </row>
+    <row r="19" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7"/>
@@ -753,9 +797,9 @@
       <c r="H19" s="7"/>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C20" s="7"/>
+      <c r="K19" s="7"/>
+    </row>
+    <row r="20" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D20" s="7"/>
       <c r="E20" s="7"/>
       <c r="F20" s="7"/>
@@ -763,9 +807,9 @@
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
-    </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C21" s="7"/>
+      <c r="K20" s="7"/>
+    </row>
+    <row r="21" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D21" s="7"/>
       <c r="E21" s="7"/>
       <c r="F21" s="7"/>
@@ -773,9 +817,9 @@
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
       <c r="J21" s="7"/>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C22" s="7"/>
+      <c r="K21" s="7"/>
+    </row>
+    <row r="22" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
       <c r="F22" s="7"/>
@@ -783,9 +827,9 @@
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
-    </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C23" s="7"/>
+      <c r="K22" s="7"/>
+    </row>
+    <row r="23" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D23" s="7"/>
       <c r="E23" s="7"/>
       <c r="F23" s="7"/>
@@ -793,9 +837,9 @@
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
       <c r="J23" s="7"/>
-    </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C24" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D24" s="7"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -803,9 +847,9 @@
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
       <c r="J24" s="7"/>
-    </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C25" s="7"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D25" s="7"/>
       <c r="E25" s="7"/>
       <c r="F25" s="7"/>
@@ -813,9 +857,9 @@
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
-    </row>
-    <row r="26" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C26" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -823,9 +867,9 @@
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
-    </row>
-    <row r="27" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C27" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D27" s="7"/>
       <c r="E27" s="7"/>
       <c r="F27" s="7"/>
@@ -833,9 +877,9 @@
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
-    </row>
-    <row r="28" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C28" s="7"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D28" s="7"/>
       <c r="E28" s="7"/>
       <c r="F28" s="7"/>
@@ -843,9 +887,9 @@
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
-    </row>
-    <row r="29" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C29" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7"/>
@@ -853,9 +897,9 @@
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
-    </row>
-    <row r="30" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C30" s="7"/>
+      <c r="K29" s="7"/>
+    </row>
+    <row r="30" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D30" s="7"/>
       <c r="E30" s="7"/>
       <c r="F30" s="7"/>
@@ -863,9 +907,9 @@
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
-    </row>
-    <row r="31" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C31" s="7"/>
+      <c r="K30" s="7"/>
+    </row>
+    <row r="31" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
       <c r="F31" s="7"/>
@@ -873,9 +917,9 @@
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
-    </row>
-    <row r="32" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C32" s="7"/>
+      <c r="K31" s="7"/>
+    </row>
+    <row r="32" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D32" s="7"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -883,9 +927,9 @@
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
       <c r="J32" s="7"/>
-    </row>
-    <row r="33" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C33" s="7"/>
+      <c r="K32" s="7"/>
+    </row>
+    <row r="33" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7"/>
@@ -893,9 +937,9 @@
       <c r="H33" s="7"/>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
-    </row>
-    <row r="34" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C34" s="7"/>
+      <c r="K33" s="7"/>
+    </row>
+    <row r="34" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D34" s="7"/>
       <c r="E34" s="7"/>
       <c r="F34" s="7"/>
@@ -903,9 +947,9 @@
       <c r="H34" s="7"/>
       <c r="I34" s="7"/>
       <c r="J34" s="7"/>
-    </row>
-    <row r="35" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C35" s="7"/>
+      <c r="K34" s="7"/>
+    </row>
+    <row r="35" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7"/>
@@ -913,9 +957,9 @@
       <c r="H35" s="7"/>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
-    </row>
-    <row r="36" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C36" s="7"/>
+      <c r="K35" s="7"/>
+    </row>
+    <row r="36" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
@@ -923,9 +967,9 @@
       <c r="H36" s="7"/>
       <c r="I36" s="7"/>
       <c r="J36" s="7"/>
-    </row>
-    <row r="37" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C37" s="7"/>
+      <c r="K36" s="7"/>
+    </row>
+    <row r="37" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7"/>
@@ -933,9 +977,9 @@
       <c r="H37" s="7"/>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
-    </row>
-    <row r="38" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C38" s="7"/>
+      <c r="K37" s="7"/>
+    </row>
+    <row r="38" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D38" s="7"/>
       <c r="E38" s="7"/>
       <c r="F38" s="7"/>
@@ -943,9 +987,9 @@
       <c r="H38" s="7"/>
       <c r="I38" s="7"/>
       <c r="J38" s="7"/>
-    </row>
-    <row r="39" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C39" s="7"/>
+      <c r="K38" s="7"/>
+    </row>
+    <row r="39" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D39" s="7"/>
       <c r="E39" s="7"/>
       <c r="F39" s="7"/>
@@ -953,9 +997,9 @@
       <c r="H39" s="7"/>
       <c r="I39" s="7"/>
       <c r="J39" s="7"/>
-    </row>
-    <row r="40" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C40" s="7"/>
+      <c r="K39" s="7"/>
+    </row>
+    <row r="40" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D40" s="7"/>
       <c r="E40" s="7"/>
       <c r="F40" s="7"/>
@@ -963,9 +1007,9 @@
       <c r="H40" s="7"/>
       <c r="I40" s="7"/>
       <c r="J40" s="7"/>
-    </row>
-    <row r="41" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C41" s="7"/>
+      <c r="K40" s="7"/>
+    </row>
+    <row r="41" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D41" s="7"/>
       <c r="E41" s="7"/>
       <c r="F41" s="7"/>
@@ -973,9 +1017,9 @@
       <c r="H41" s="7"/>
       <c r="I41" s="7"/>
       <c r="J41" s="7"/>
-    </row>
-    <row r="42" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C42" s="7"/>
+      <c r="K41" s="7"/>
+    </row>
+    <row r="42" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
@@ -983,9 +1027,9 @@
       <c r="H42" s="7"/>
       <c r="I42" s="7"/>
       <c r="J42" s="7"/>
-    </row>
-    <row r="43" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C43" s="7"/>
+      <c r="K42" s="7"/>
+    </row>
+    <row r="43" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -993,9 +1037,9 @@
       <c r="H43" s="7"/>
       <c r="I43" s="7"/>
       <c r="J43" s="7"/>
-    </row>
-    <row r="44" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C44" s="7"/>
+      <c r="K43" s="7"/>
+    </row>
+    <row r="44" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D44" s="7"/>
       <c r="E44" s="7"/>
       <c r="F44" s="7"/>
@@ -1003,9 +1047,9 @@
       <c r="H44" s="7"/>
       <c r="I44" s="7"/>
       <c r="J44" s="7"/>
-    </row>
-    <row r="45" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C45" s="7"/>
+      <c r="K44" s="7"/>
+    </row>
+    <row r="45" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7"/>
@@ -1013,9 +1057,9 @@
       <c r="H45" s="7"/>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
-    </row>
-    <row r="46" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C46" s="7"/>
+      <c r="K45" s="7"/>
+    </row>
+    <row r="46" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D46" s="7"/>
       <c r="E46" s="7"/>
       <c r="F46" s="7"/>
@@ -1023,9 +1067,9 @@
       <c r="H46" s="7"/>
       <c r="I46" s="7"/>
       <c r="J46" s="7"/>
-    </row>
-    <row r="47" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C47" s="7"/>
+      <c r="K46" s="7"/>
+    </row>
+    <row r="47" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7"/>
@@ -1033,9 +1077,9 @@
       <c r="H47" s="7"/>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
-    </row>
-    <row r="48" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C48" s="7"/>
+      <c r="K47" s="7"/>
+    </row>
+    <row r="48" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="7"/>
@@ -1043,9 +1087,9 @@
       <c r="H48" s="7"/>
       <c r="I48" s="7"/>
       <c r="J48" s="7"/>
-    </row>
-    <row r="49" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C49" s="7"/>
+      <c r="K48" s="7"/>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
@@ -1053,9 +1097,9 @@
       <c r="H49" s="7"/>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
-    </row>
-    <row r="50" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C50" s="7"/>
+      <c r="K49" s="7"/>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D50" s="7"/>
       <c r="E50" s="7"/>
       <c r="F50" s="7"/>
@@ -1063,9 +1107,9 @@
       <c r="H50" s="7"/>
       <c r="I50" s="7"/>
       <c r="J50" s="7"/>
-    </row>
-    <row r="51" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C51" s="7"/>
+      <c r="K50" s="7"/>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D51" s="7"/>
       <c r="E51" s="7"/>
       <c r="F51" s="7"/>
@@ -1073,9 +1117,9 @@
       <c r="H51" s="7"/>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
-    </row>
-    <row r="52" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C52" s="7"/>
+      <c r="K51" s="7"/>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D52" s="7"/>
       <c r="E52" s="7"/>
       <c r="F52" s="7"/>
@@ -1083,9 +1127,9 @@
       <c r="H52" s="7"/>
       <c r="I52" s="7"/>
       <c r="J52" s="7"/>
-    </row>
-    <row r="53" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C53" s="7"/>
+      <c r="K52" s="7"/>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D53" s="7"/>
       <c r="E53" s="7"/>
       <c r="F53" s="7"/>
@@ -1093,9 +1137,9 @@
       <c r="H53" s="7"/>
       <c r="I53" s="7"/>
       <c r="J53" s="7"/>
-    </row>
-    <row r="54" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C54" s="7"/>
+      <c r="K53" s="7"/>
+    </row>
+    <row r="54" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D54" s="7"/>
       <c r="E54" s="7"/>
       <c r="F54" s="7"/>
@@ -1103,9 +1147,9 @@
       <c r="H54" s="7"/>
       <c r="I54" s="7"/>
       <c r="J54" s="7"/>
-    </row>
-    <row r="55" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C55" s="7"/>
+      <c r="K54" s="7"/>
+    </row>
+    <row r="55" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D55" s="7"/>
       <c r="E55" s="7"/>
       <c r="F55" s="7"/>
@@ -1113,9 +1157,9 @@
       <c r="H55" s="7"/>
       <c r="I55" s="7"/>
       <c r="J55" s="7"/>
-    </row>
-    <row r="56" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C56" s="7"/>
+      <c r="K55" s="7"/>
+    </row>
+    <row r="56" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D56" s="7"/>
       <c r="E56" s="7"/>
       <c r="F56" s="7"/>
@@ -1123,9 +1167,9 @@
       <c r="H56" s="7"/>
       <c r="I56" s="7"/>
       <c r="J56" s="7"/>
-    </row>
-    <row r="57" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C57" s="7"/>
+      <c r="K56" s="7"/>
+    </row>
+    <row r="57" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D57" s="7"/>
       <c r="E57" s="7"/>
       <c r="F57" s="7"/>
@@ -1133,9 +1177,9 @@
       <c r="H57" s="7"/>
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
-    </row>
-    <row r="58" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C58" s="7"/>
+      <c r="K57" s="7"/>
+    </row>
+    <row r="58" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D58" s="7"/>
       <c r="E58" s="7"/>
       <c r="F58" s="7"/>
@@ -1143,9 +1187,9 @@
       <c r="H58" s="7"/>
       <c r="I58" s="7"/>
       <c r="J58" s="7"/>
-    </row>
-    <row r="59" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C59" s="7"/>
+      <c r="K58" s="7"/>
+    </row>
+    <row r="59" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D59" s="7"/>
       <c r="E59" s="7"/>
       <c r="F59" s="7"/>
@@ -1153,9 +1197,9 @@
       <c r="H59" s="7"/>
       <c r="I59" s="7"/>
       <c r="J59" s="7"/>
-    </row>
-    <row r="60" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C60" s="7"/>
+      <c r="K59" s="7"/>
+    </row>
+    <row r="60" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D60" s="7"/>
       <c r="E60" s="7"/>
       <c r="F60" s="7"/>
@@ -1163,9 +1207,9 @@
       <c r="H60" s="7"/>
       <c r="I60" s="7"/>
       <c r="J60" s="7"/>
-    </row>
-    <row r="61" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C61" s="7"/>
+      <c r="K60" s="7"/>
+    </row>
+    <row r="61" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D61" s="7"/>
       <c r="E61" s="7"/>
       <c r="F61" s="7"/>
@@ -1173,9 +1217,9 @@
       <c r="H61" s="7"/>
       <c r="I61" s="7"/>
       <c r="J61" s="7"/>
-    </row>
-    <row r="62" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C62" s="7"/>
+      <c r="K61" s="7"/>
+    </row>
+    <row r="62" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D62" s="7"/>
       <c r="E62" s="7"/>
       <c r="F62" s="7"/>
@@ -1183,9 +1227,9 @@
       <c r="H62" s="7"/>
       <c r="I62" s="7"/>
       <c r="J62" s="7"/>
-    </row>
-    <row r="63" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C63" s="7"/>
+      <c r="K62" s="7"/>
+    </row>
+    <row r="63" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
       <c r="F63" s="7"/>
@@ -1193,9 +1237,9 @@
       <c r="H63" s="7"/>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
-    </row>
-    <row r="64" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C64" s="7"/>
+      <c r="K63" s="7"/>
+    </row>
+    <row r="64" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D64" s="7"/>
       <c r="E64" s="7"/>
       <c r="F64" s="7"/>
@@ -1203,9 +1247,9 @@
       <c r="H64" s="7"/>
       <c r="I64" s="7"/>
       <c r="J64" s="7"/>
-    </row>
-    <row r="65" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C65" s="7"/>
+      <c r="K64" s="7"/>
+    </row>
+    <row r="65" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D65" s="7"/>
       <c r="E65" s="7"/>
       <c r="F65" s="7"/>
@@ -1213,9 +1257,9 @@
       <c r="H65" s="7"/>
       <c r="I65" s="7"/>
       <c r="J65" s="7"/>
-    </row>
-    <row r="66" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C66" s="7"/>
+      <c r="K65" s="7"/>
+    </row>
+    <row r="66" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D66" s="7"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -1223,9 +1267,9 @@
       <c r="H66" s="7"/>
       <c r="I66" s="7"/>
       <c r="J66" s="7"/>
-    </row>
-    <row r="67" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C67" s="7"/>
+      <c r="K66" s="7"/>
+    </row>
+    <row r="67" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D67" s="7"/>
       <c r="E67" s="7"/>
       <c r="F67" s="7"/>
@@ -1233,9 +1277,9 @@
       <c r="H67" s="7"/>
       <c r="I67" s="7"/>
       <c r="J67" s="7"/>
-    </row>
-    <row r="68" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C68" s="7"/>
+      <c r="K67" s="7"/>
+    </row>
+    <row r="68" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D68" s="7"/>
       <c r="E68" s="7"/>
       <c r="F68" s="7"/>
@@ -1243,9 +1287,9 @@
       <c r="H68" s="7"/>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
-    </row>
-    <row r="69" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C69" s="7"/>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D69" s="7"/>
       <c r="E69" s="7"/>
       <c r="F69" s="7"/>
@@ -1253,9 +1297,9 @@
       <c r="H69" s="7"/>
       <c r="I69" s="7"/>
       <c r="J69" s="7"/>
-    </row>
-    <row r="70" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C70" s="7"/>
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D70" s="7"/>
       <c r="E70" s="7"/>
       <c r="F70" s="7"/>
@@ -1263,9 +1307,9 @@
       <c r="H70" s="7"/>
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
-    </row>
-    <row r="71" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C71" s="7"/>
+      <c r="K70" s="7"/>
+    </row>
+    <row r="71" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D71" s="7"/>
       <c r="E71" s="7"/>
       <c r="F71" s="7"/>
@@ -1273,9 +1317,9 @@
       <c r="H71" s="7"/>
       <c r="I71" s="7"/>
       <c r="J71" s="7"/>
-    </row>
-    <row r="72" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C72" s="7"/>
+      <c r="K71" s="7"/>
+    </row>
+    <row r="72" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D72" s="7"/>
       <c r="E72" s="7"/>
       <c r="F72" s="7"/>
@@ -1283,9 +1327,9 @@
       <c r="H72" s="7"/>
       <c r="I72" s="7"/>
       <c r="J72" s="7"/>
-    </row>
-    <row r="73" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C73" s="7"/>
+      <c r="K72" s="7"/>
+    </row>
+    <row r="73" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D73" s="7"/>
       <c r="E73" s="7"/>
       <c r="F73" s="7"/>
@@ -1293,9 +1337,9 @@
       <c r="H73" s="7"/>
       <c r="I73" s="7"/>
       <c r="J73" s="7"/>
-    </row>
-    <row r="74" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C74" s="7"/>
+      <c r="K73" s="7"/>
+    </row>
+    <row r="74" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D74" s="7"/>
       <c r="E74" s="7"/>
       <c r="F74" s="7"/>
@@ -1303,9 +1347,9 @@
       <c r="H74" s="7"/>
       <c r="I74" s="7"/>
       <c r="J74" s="7"/>
-    </row>
-    <row r="75" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C75" s="7"/>
+      <c r="K74" s="7"/>
+    </row>
+    <row r="75" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D75" s="7"/>
       <c r="E75" s="7"/>
       <c r="F75" s="7"/>
@@ -1313,9 +1357,9 @@
       <c r="H75" s="7"/>
       <c r="I75" s="7"/>
       <c r="J75" s="7"/>
-    </row>
-    <row r="76" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C76" s="7"/>
+      <c r="K75" s="7"/>
+    </row>
+    <row r="76" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D76" s="7"/>
       <c r="E76" s="7"/>
       <c r="F76" s="7"/>
@@ -1323,9 +1367,9 @@
       <c r="H76" s="7"/>
       <c r="I76" s="7"/>
       <c r="J76" s="7"/>
-    </row>
-    <row r="77" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C77" s="7"/>
+      <c r="K76" s="7"/>
+    </row>
+    <row r="77" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D77" s="7"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
@@ -1333,9 +1377,9 @@
       <c r="H77" s="7"/>
       <c r="I77" s="7"/>
       <c r="J77" s="7"/>
-    </row>
-    <row r="78" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C78" s="7"/>
+      <c r="K77" s="7"/>
+    </row>
+    <row r="78" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D78" s="7"/>
       <c r="E78" s="7"/>
       <c r="F78" s="7"/>
@@ -1343,9 +1387,9 @@
       <c r="H78" s="7"/>
       <c r="I78" s="7"/>
       <c r="J78" s="7"/>
-    </row>
-    <row r="79" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C79" s="7"/>
+      <c r="K78" s="7"/>
+    </row>
+    <row r="79" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D79" s="7"/>
       <c r="E79" s="7"/>
       <c r="F79" s="7"/>
@@ -1353,9 +1397,9 @@
       <c r="H79" s="7"/>
       <c r="I79" s="7"/>
       <c r="J79" s="7"/>
-    </row>
-    <row r="80" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C80" s="7"/>
+      <c r="K79" s="7"/>
+    </row>
+    <row r="80" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D80" s="7"/>
       <c r="E80" s="7"/>
       <c r="F80" s="7"/>
@@ -1363,9 +1407,9 @@
       <c r="H80" s="7"/>
       <c r="I80" s="7"/>
       <c r="J80" s="7"/>
-    </row>
-    <row r="81" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C81" s="7"/>
+      <c r="K80" s="7"/>
+    </row>
+    <row r="81" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D81" s="7"/>
       <c r="E81" s="7"/>
       <c r="F81" s="7"/>
@@ -1373,9 +1417,9 @@
       <c r="H81" s="7"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
-    </row>
-    <row r="82" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C82" s="7"/>
+      <c r="K81" s="7"/>
+    </row>
+    <row r="82" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D82" s="7"/>
       <c r="E82" s="7"/>
       <c r="F82" s="7"/>
@@ -1383,9 +1427,9 @@
       <c r="H82" s="7"/>
       <c r="I82" s="7"/>
       <c r="J82" s="7"/>
-    </row>
-    <row r="83" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C83" s="7"/>
+      <c r="K82" s="7"/>
+    </row>
+    <row r="83" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D83" s="7"/>
       <c r="E83" s="7"/>
       <c r="F83" s="7"/>
@@ -1393,9 +1437,9 @@
       <c r="H83" s="7"/>
       <c r="I83" s="7"/>
       <c r="J83" s="7"/>
-    </row>
-    <row r="84" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C84" s="7"/>
+      <c r="K83" s="7"/>
+    </row>
+    <row r="84" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D84" s="7"/>
       <c r="E84" s="7"/>
       <c r="F84" s="7"/>
@@ -1403,9 +1447,9 @@
       <c r="H84" s="7"/>
       <c r="I84" s="7"/>
       <c r="J84" s="7"/>
-    </row>
-    <row r="85" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C85" s="7"/>
+      <c r="K84" s="7"/>
+    </row>
+    <row r="85" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D85" s="7"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -1413,9 +1457,9 @@
       <c r="H85" s="7"/>
       <c r="I85" s="7"/>
       <c r="J85" s="7"/>
-    </row>
-    <row r="86" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C86" s="7"/>
+      <c r="K85" s="7"/>
+    </row>
+    <row r="86" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D86" s="7"/>
       <c r="E86" s="7"/>
       <c r="F86" s="7"/>
@@ -1423,9 +1467,9 @@
       <c r="H86" s="7"/>
       <c r="I86" s="7"/>
       <c r="J86" s="7"/>
-    </row>
-    <row r="87" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C87" s="7"/>
+      <c r="K86" s="7"/>
+    </row>
+    <row r="87" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D87" s="7"/>
       <c r="E87" s="7"/>
       <c r="F87" s="7"/>
@@ -1433,9 +1477,9 @@
       <c r="H87" s="7"/>
       <c r="I87" s="7"/>
       <c r="J87" s="7"/>
-    </row>
-    <row r="88" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C88" s="7"/>
+      <c r="K87" s="7"/>
+    </row>
+    <row r="88" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D88" s="7"/>
       <c r="E88" s="7"/>
       <c r="F88" s="7"/>
@@ -1443,9 +1487,9 @@
       <c r="H88" s="7"/>
       <c r="I88" s="7"/>
       <c r="J88" s="7"/>
-    </row>
-    <row r="89" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C89" s="7"/>
+      <c r="K88" s="7"/>
+    </row>
+    <row r="89" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D89" s="7"/>
       <c r="E89" s="7"/>
       <c r="F89" s="7"/>
@@ -1453,9 +1497,9 @@
       <c r="H89" s="7"/>
       <c r="I89" s="7"/>
       <c r="J89" s="7"/>
-    </row>
-    <row r="90" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C90" s="7"/>
+      <c r="K89" s="7"/>
+    </row>
+    <row r="90" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D90" s="7"/>
       <c r="E90" s="7"/>
       <c r="F90" s="7"/>
@@ -1463,9 +1507,9 @@
       <c r="H90" s="7"/>
       <c r="I90" s="7"/>
       <c r="J90" s="7"/>
-    </row>
-    <row r="91" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C91" s="7"/>
+      <c r="K90" s="7"/>
+    </row>
+    <row r="91" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D91" s="7"/>
       <c r="E91" s="7"/>
       <c r="F91" s="7"/>
@@ -1473,9 +1517,9 @@
       <c r="H91" s="7"/>
       <c r="I91" s="7"/>
       <c r="J91" s="7"/>
-    </row>
-    <row r="92" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C92" s="7"/>
+      <c r="K91" s="7"/>
+    </row>
+    <row r="92" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D92" s="7"/>
       <c r="E92" s="7"/>
       <c r="F92" s="7"/>
@@ -1483,9 +1527,9 @@
       <c r="H92" s="7"/>
       <c r="I92" s="7"/>
       <c r="J92" s="7"/>
-    </row>
-    <row r="93" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C93" s="7"/>
+      <c r="K92" s="7"/>
+    </row>
+    <row r="93" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D93" s="7"/>
       <c r="E93" s="7"/>
       <c r="F93" s="7"/>
@@ -1493,9 +1537,9 @@
       <c r="H93" s="7"/>
       <c r="I93" s="7"/>
       <c r="J93" s="7"/>
-    </row>
-    <row r="94" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C94" s="7"/>
+      <c r="K93" s="7"/>
+    </row>
+    <row r="94" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D94" s="7"/>
       <c r="E94" s="7"/>
       <c r="F94" s="7"/>
@@ -1503,9 +1547,9 @@
       <c r="H94" s="7"/>
       <c r="I94" s="7"/>
       <c r="J94" s="7"/>
-    </row>
-    <row r="95" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C95" s="7"/>
+      <c r="K94" s="7"/>
+    </row>
+    <row r="95" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D95" s="7"/>
       <c r="E95" s="7"/>
       <c r="F95" s="7"/>
@@ -1513,9 +1557,9 @@
       <c r="H95" s="7"/>
       <c r="I95" s="7"/>
       <c r="J95" s="7"/>
-    </row>
-    <row r="96" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C96" s="7"/>
+      <c r="K95" s="7"/>
+    </row>
+    <row r="96" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D96" s="7"/>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
@@ -1523,9 +1567,9 @@
       <c r="H96" s="7"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
-    </row>
-    <row r="97" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C97" s="7"/>
+      <c r="K96" s="7"/>
+    </row>
+    <row r="97" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D97" s="7"/>
       <c r="E97" s="7"/>
       <c r="F97" s="7"/>
@@ -1533,9 +1577,9 @@
       <c r="H97" s="7"/>
       <c r="I97" s="7"/>
       <c r="J97" s="7"/>
-    </row>
-    <row r="98" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C98" s="7"/>
+      <c r="K97" s="7"/>
+    </row>
+    <row r="98" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D98" s="7"/>
       <c r="E98" s="7"/>
       <c r="F98" s="7"/>
@@ -1543,9 +1587,9 @@
       <c r="H98" s="7"/>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
-    </row>
-    <row r="99" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C99" s="7"/>
+      <c r="K98" s="7"/>
+    </row>
+    <row r="99" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D99" s="7"/>
       <c r="E99" s="7"/>
       <c r="F99" s="7"/>
@@ -1553,9 +1597,9 @@
       <c r="H99" s="7"/>
       <c r="I99" s="7"/>
       <c r="J99" s="7"/>
-    </row>
-    <row r="100" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C100" s="7"/>
+      <c r="K99" s="7"/>
+    </row>
+    <row r="100" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D100" s="7"/>
       <c r="E100" s="7"/>
       <c r="F100" s="7"/>
@@ -1563,9 +1607,9 @@
       <c r="H100" s="7"/>
       <c r="I100" s="7"/>
       <c r="J100" s="7"/>
-    </row>
-    <row r="101" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C101" s="7"/>
+      <c r="K100" s="7"/>
+    </row>
+    <row r="101" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D101" s="7"/>
       <c r="E101" s="7"/>
       <c r="F101" s="7"/>
@@ -1573,9 +1617,9 @@
       <c r="H101" s="7"/>
       <c r="I101" s="7"/>
       <c r="J101" s="7"/>
-    </row>
-    <row r="102" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C102" s="7"/>
+      <c r="K101" s="7"/>
+    </row>
+    <row r="102" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D102" s="7"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -1583,9 +1627,9 @@
       <c r="H102" s="7"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
-    </row>
-    <row r="103" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C103" s="7"/>
+      <c r="K102" s="7"/>
+    </row>
+    <row r="103" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D103" s="7"/>
       <c r="E103" s="7"/>
       <c r="F103" s="7"/>
@@ -1593,9 +1637,9 @@
       <c r="H103" s="7"/>
       <c r="I103" s="7"/>
       <c r="J103" s="7"/>
-    </row>
-    <row r="104" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C104" s="7"/>
+      <c r="K103" s="7"/>
+    </row>
+    <row r="104" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D104" s="7"/>
       <c r="E104" s="7"/>
       <c r="F104" s="7"/>
@@ -1603,9 +1647,9 @@
       <c r="H104" s="7"/>
       <c r="I104" s="7"/>
       <c r="J104" s="7"/>
-    </row>
-    <row r="105" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C105" s="7"/>
+      <c r="K104" s="7"/>
+    </row>
+    <row r="105" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D105" s="7"/>
       <c r="E105" s="7"/>
       <c r="F105" s="7"/>
@@ -1613,9 +1657,9 @@
       <c r="H105" s="7"/>
       <c r="I105" s="7"/>
       <c r="J105" s="7"/>
-    </row>
-    <row r="106" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C106" s="7"/>
+      <c r="K105" s="7"/>
+    </row>
+    <row r="106" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D106" s="7"/>
       <c r="E106" s="7"/>
       <c r="F106" s="7"/>
@@ -1623,9 +1667,9 @@
       <c r="H106" s="7"/>
       <c r="I106" s="7"/>
       <c r="J106" s="7"/>
-    </row>
-    <row r="107" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C107" s="7"/>
+      <c r="K106" s="7"/>
+    </row>
+    <row r="107" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D107" s="7"/>
       <c r="E107" s="7"/>
       <c r="F107" s="7"/>
@@ -1633,9 +1677,9 @@
       <c r="H107" s="7"/>
       <c r="I107" s="7"/>
       <c r="J107" s="7"/>
-    </row>
-    <row r="108" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C108" s="7"/>
+      <c r="K107" s="7"/>
+    </row>
+    <row r="108" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D108" s="7"/>
       <c r="E108" s="7"/>
       <c r="F108" s="7"/>
@@ -1643,9 +1687,9 @@
       <c r="H108" s="7"/>
       <c r="I108" s="7"/>
       <c r="J108" s="7"/>
-    </row>
-    <row r="109" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C109" s="7"/>
+      <c r="K108" s="7"/>
+    </row>
+    <row r="109" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D109" s="7"/>
       <c r="E109" s="7"/>
       <c r="F109" s="7"/>
@@ -1653,9 +1697,9 @@
       <c r="H109" s="7"/>
       <c r="I109" s="7"/>
       <c r="J109" s="7"/>
-    </row>
-    <row r="110" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C110" s="7"/>
+      <c r="K109" s="7"/>
+    </row>
+    <row r="110" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D110" s="7"/>
       <c r="E110" s="7"/>
       <c r="F110" s="7"/>
@@ -1663,9 +1707,9 @@
       <c r="H110" s="7"/>
       <c r="I110" s="7"/>
       <c r="J110" s="7"/>
-    </row>
-    <row r="111" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C111" s="7"/>
+      <c r="K110" s="7"/>
+    </row>
+    <row r="111" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D111" s="7"/>
       <c r="E111" s="7"/>
       <c r="F111" s="7"/>
@@ -1673,9 +1717,9 @@
       <c r="H111" s="7"/>
       <c r="I111" s="7"/>
       <c r="J111" s="7"/>
-    </row>
-    <row r="112" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C112" s="7"/>
+      <c r="K111" s="7"/>
+    </row>
+    <row r="112" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D112" s="7"/>
       <c r="E112" s="7"/>
       <c r="F112" s="7"/>
@@ -1683,9 +1727,9 @@
       <c r="H112" s="7"/>
       <c r="I112" s="7"/>
       <c r="J112" s="7"/>
-    </row>
-    <row r="113" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C113" s="7"/>
+      <c r="K112" s="7"/>
+    </row>
+    <row r="113" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D113" s="7"/>
       <c r="E113" s="7"/>
       <c r="F113" s="7"/>
@@ -1693,9 +1737,9 @@
       <c r="H113" s="7"/>
       <c r="I113" s="7"/>
       <c r="J113" s="7"/>
-    </row>
-    <row r="114" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C114" s="7"/>
+      <c r="K113" s="7"/>
+    </row>
+    <row r="114" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D114" s="7"/>
       <c r="E114" s="7"/>
       <c r="F114" s="7"/>
@@ -1703,9 +1747,9 @@
       <c r="H114" s="7"/>
       <c r="I114" s="7"/>
       <c r="J114" s="7"/>
-    </row>
-    <row r="115" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C115" s="7"/>
+      <c r="K114" s="7"/>
+    </row>
+    <row r="115" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D115" s="7"/>
       <c r="E115" s="7"/>
       <c r="F115" s="7"/>
@@ -1713,9 +1757,9 @@
       <c r="H115" s="7"/>
       <c r="I115" s="7"/>
       <c r="J115" s="7"/>
-    </row>
-    <row r="116" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C116" s="7"/>
+      <c r="K115" s="7"/>
+    </row>
+    <row r="116" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D116" s="7"/>
       <c r="E116" s="7"/>
       <c r="F116" s="7"/>
@@ -1723,9 +1767,9 @@
       <c r="H116" s="7"/>
       <c r="I116" s="7"/>
       <c r="J116" s="7"/>
-    </row>
-    <row r="117" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C117" s="7"/>
+      <c r="K116" s="7"/>
+    </row>
+    <row r="117" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D117" s="7"/>
       <c r="E117" s="7"/>
       <c r="F117" s="7"/>
@@ -1733,9 +1777,9 @@
       <c r="H117" s="7"/>
       <c r="I117" s="7"/>
       <c r="J117" s="7"/>
-    </row>
-    <row r="118" spans="3:10" x14ac:dyDescent="0.2">
-      <c r="C118" s="7"/>
+      <c r="K117" s="7"/>
+    </row>
+    <row r="118" spans="4:11" x14ac:dyDescent="0.2">
       <c r="D118" s="7"/>
       <c r="E118" s="7"/>
       <c r="F118" s="7"/>
@@ -1743,6 +1787,7 @@
       <c r="H118" s="7"/>
       <c r="I118" s="7"/>
       <c r="J118" s="7"/>
+      <c r="K118" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Test Private Method in Java Private method can be used in the self class, not in outer class
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -147,7 +147,9 @@
   <si>
     <t>1. private int N = 0;
  &lt;-- holds index of next available cell 
-in the items array</t>
+in the items array
+2. Test Private Method in Java
+Private method can be used in the self class, not in outer class</t>
   </si>
 </sst>
 </file>
@@ -524,8 +526,8 @@
   <sheetPr codeName="Sheet1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
loitering avoid in pop(), java array
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -210,7 +210,8 @@
        public void remove()    
        {                  }
 }
-2: Question: avoid loitering ???</t>
+2: Question: avoid loitering ???
+     See Readme.Md</t>
   </si>
 </sst>
 </file>
@@ -588,7 +589,7 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -733,7 +734,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="176" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" ht="192" x14ac:dyDescent="0.2">
       <c r="B6" s="3">
         <v>4</v>
       </c>

</xml_diff>

<commit_message>
Python 2 player win 15
</commit_message>
<xml_diff>
--- a/Algs4.xlsx
+++ b/Algs4.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="44">
   <si>
     <t>Topic</t>
   </si>
@@ -218,6 +218,29 @@
   </si>
   <si>
     <t>LinkedListSean.java</t>
+  </si>
+  <si>
+    <t>1. http://www.geeksforgeeks.org/linked-list-set-2-inserting-a-node/</t>
+  </si>
+  <si>
+    <t>1. Append(): If the linked List is empty, tail = null.</t>
+  </si>
+  <si>
+    <t>Python two players win 15</t>
+  </si>
+  <si>
+    <t># if scores of two players are same and their scores are just 1 point less
+    # than the gamePoint, deuce condition occurs.
+    # if deuce condition occurs, gamePoint needs to incremented by 1</t>
+  </si>
+  <si>
+    <t>if scoreA == scoreB and scoreA == gamePoint - 1:
+        gamePoint = gamePoint + 1</t>
+  </si>
+  <si>
+    <t>while scoreA != gamePoint and scoreB != gamePoint:
+# Check deuce condition and handle it. Update gamePoint if required
+gamePoint = checkAndHandleDeuce(scoreA, scoreB, gamePoint)</t>
   </si>
 </sst>
 </file>
@@ -598,7 +621,7 @@
   <dimension ref="A1:K117"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -779,7 +802,9 @@
         <v>36</v>
       </c>
       <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="E7" s="7" t="s">
+        <v>39</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="7" t="s">
         <v>37</v>
@@ -789,14 +814,30 @@
       </c>
       <c r="I7" s="7"/>
       <c r="J7" s="7"/>
-      <c r="K7" s="7"/>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
+      <c r="K7" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="112" x14ac:dyDescent="0.2">
+      <c r="B8" s="3">
+        <v>6</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>43</v>
+      </c>
       <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
+      <c r="H8" s="8">
+        <v>42927</v>
+      </c>
       <c r="I8" s="7"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>

</xml_diff>